<commit_message>
Fixed name of commodity and other small issues
</commit_message>
<xml_diff>
--- a/Add Sectors/new_activities.xlsx
+++ b/Add Sectors/new_activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\Add Sectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8518D4A8-9BA8-4108-87C6-EAD3A9D442C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFE2746-3A38-4BAB-8F5B-DBFE2C5A0E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indeces" sheetId="1" r:id="rId1"/>
@@ -21,25 +21,12 @@
     <sheet name="output_from" sheetId="6" r:id="rId6"/>
     <sheet name="units" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="1491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="1491">
   <si>
     <t>EU27+UK</t>
   </si>
@@ -4508,19 +4495,16 @@
     <t>Extension</t>
   </si>
   <si>
-    <t>Raw silicon</t>
-  </si>
-  <si>
     <t>unit</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4579,12 +4563,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4889,7 +4872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -11594,7 +11579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -11677,16 +11662,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="86.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -11893,36 +11877,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
-        <f>SUM(B4:B15)+SUM(input_from!D4:D85)</f>
-        <v>0.99999999999999867</v>
-      </c>
-      <c r="C17" s="2">
-        <f>SUM(C4:C15)+SUM(input_from!E4:E85)</f>
-        <v>0.99999999999999967</v>
-      </c>
-      <c r="D17" s="2">
-        <f>SUM(D4:D15)+SUM(input_from!F4:F85)</f>
-        <v>1.0000000000000002</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B85">
-        <v>0</v>
-      </c>
-      <c r="C85">
-        <v>7.0165344315910464E-3</v>
-      </c>
-      <c r="D85">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>indeces!$G$1:$G$12</xm:f>
@@ -12000,9 +11959,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="58.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
@@ -13494,7 +13461,7 @@
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>1489</v>
+        <v>322</v>
       </c>
       <c r="D76">
         <v>3.0404859261270081E-2</v>
@@ -13514,7 +13481,7 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>1489</v>
+        <v>322</v>
       </c>
       <c r="D77">
         <v>3.0711979051787968E-3</v>
@@ -13534,7 +13501,7 @@
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>1489</v>
+        <v>322</v>
       </c>
       <c r="D78">
         <v>2.764078114660918E-3</v>
@@ -13554,7 +13521,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>1489</v>
+        <v>322</v>
       </c>
       <c r="D79">
         <v>2.1498385336251578E-3</v>
@@ -13804,28 +13771,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1486</v>
+        <v>1485</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1490</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1484</v>
       </c>
+      <c r="B3" t="s">
+        <v>1490</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update all the inventories, modify new_commodities in Add sector, run 2. Add sectors
</commit_message>
<xml_diff>
--- a/Add Sectors/new_activities.xlsx
+++ b/Add Sectors/new_activities.xlsx
@@ -10582,7 +10582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10997,7 +10997,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -11011,19 +11011,19 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.04149625757138736</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.005330264331415682</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.004681043959697958</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -11033,23 +11033,23 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Electrical machinery and apparatus n.e.c. (31)</t>
+          <t>Copper ores and concentrates</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>0.04149625757138736</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1153736868271792</v>
+        <v>0.03988348337202882</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04891956955786517</v>
+        <v>0.0319845187476479</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -11059,17 +11059,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Electrical machinery and apparatus n.e.c. (31)</t>
+          <t>Dysprosium</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.08534250793192952</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1479530208997053</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.07876710849731904</v>
+        <v>0.0009760668273203698</v>
       </c>
     </row>
     <row r="20">
@@ -11085,17 +11085,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Electricity by Geothermal</t>
+          <t>Electrical machinery and apparatus n.e.c. (31)</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9.013925911896396e-07</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>0.1100434224957636</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.04423852559816721</v>
       </c>
     </row>
     <row r="21">
@@ -11111,23 +11111,23 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Electricity by Geothermal</t>
+          <t>Electrical machinery and apparatus n.e.c. (31)</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.0007162333062425288</v>
+        <v>0.08534250793192952</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>0.1080695375276765</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.05250736500058427</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -11141,7 +11141,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4.049788969545348e-05</v>
+        <v>9.013925911896396e-07</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -11153,7 +11153,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -11167,7 +11167,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.000106608893904089</v>
+        <v>0.0007162333062425288</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -11179,7 +11179,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -11189,11 +11189,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Electricity by biomass and waste</t>
+          <t>Electricity by Geothermal</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.0007214659766193121</v>
+        <v>4.049788969545348e-05</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -11205,7 +11205,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -11215,11 +11215,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Electricity by biomass and waste</t>
+          <t>Electricity by Geothermal</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.008061740824487466</v>
+        <v>0.000106608893904089</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -11231,7 +11231,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -11245,7 +11245,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.0001798349750493596</v>
+        <v>0.0007214659766193121</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -11257,7 +11257,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -11271,7 +11271,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.0004162510880805905</v>
+        <v>0.008061740824487466</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -11283,7 +11283,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -11293,11 +11293,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Electricity by coal</t>
+          <t>Electricity by biomass and waste</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.03349049032478704</v>
+        <v>0.0001798349750493596</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -11309,7 +11309,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -11319,11 +11319,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Electricity by coal</t>
+          <t>Electricity by biomass and waste</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.0287553326338111</v>
+        <v>0.0004162510880805905</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -11335,7 +11335,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -11349,7 +11349,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.002689029218752533</v>
+        <v>0.03349049032478704</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -11361,7 +11361,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -11375,7 +11375,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.006148045334480371</v>
+        <v>0.0287553326338111</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -11387,7 +11387,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -11397,11 +11397,11 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Electricity by gas</t>
+          <t>Electricity by coal</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.001363508449243723</v>
+        <v>0.002689029218752533</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -11413,7 +11413,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -11423,11 +11423,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Electricity by gas</t>
+          <t>Electricity by coal</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.02925694622314124</v>
+        <v>0.006148045334480371</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -11439,7 +11439,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -11453,7 +11453,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.00294650311108225</v>
+        <v>0.001363508449243723</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -11465,7 +11465,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -11479,7 +11479,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.008672240431651851</v>
+        <v>0.02925694622314124</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -11491,7 +11491,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -11501,11 +11501,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Electricity by hydro</t>
+          <t>Electricity by gas</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.009035728074778019</v>
+        <v>0.00294650311108225</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -11517,7 +11517,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -11527,11 +11527,11 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Electricity by hydro</t>
+          <t>Electricity by gas</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.02352282509887464</v>
+        <v>0.008672240431651851</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -11543,7 +11543,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -11557,7 +11557,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.001671891903499809</v>
+        <v>0.009035728074778019</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -11569,7 +11569,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -11583,7 +11583,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.001660926978702575</v>
+        <v>0.02352282509887464</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -11595,7 +11595,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -11605,11 +11605,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Electricity by nuclear</t>
+          <t>Electricity by hydro</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.002077268600879473</v>
+        <v>0.001671891903499809</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -11621,7 +11621,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -11631,11 +11631,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Electricity by nuclear</t>
+          <t>Electricity by hydro</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.03361338413607041</v>
+        <v>0.001660926978702575</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -11647,7 +11647,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -11661,7 +11661,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.0005593500890241802</v>
+        <v>0.002077268600879473</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -11673,7 +11673,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -11687,7 +11687,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.004618804327589211</v>
+        <v>0.03361338413607041</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -11699,7 +11699,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -11709,11 +11709,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Electricity by petroleum and other oil derivatives</t>
+          <t>Electricity by nuclear</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>7.46425176912317e-05</v>
+        <v>0.0005593500890241802</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -11725,7 +11725,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -11735,11 +11735,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Electricity by petroleum and other oil derivatives</t>
+          <t>Electricity by nuclear</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.002124700337705981</v>
+        <v>0.004618804327589211</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -11751,7 +11751,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -11765,7 +11765,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.000582883958819887</v>
+        <v>7.46425176912317e-05</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -11777,7 +11777,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -11791,7 +11791,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.0002083531209825955</v>
+        <v>0.002124700337705981</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -11803,7 +11803,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -11813,11 +11813,11 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Electricity by solar photovoltaic</t>
+          <t>Electricity by petroleum and other oil derivatives</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.001280920696696709</v>
+        <v>0.000582883958819887</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -11829,7 +11829,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -11839,11 +11839,11 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Electricity by solar photovoltaic</t>
+          <t>Electricity by petroleum and other oil derivatives</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.004991689392707744</v>
+        <v>0.0002083531209825955</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -11855,7 +11855,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -11869,7 +11869,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.0001412315744681418</v>
+        <v>0.001280920696696709</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -11881,7 +11881,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -11895,7 +11895,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.0004632706091568247</v>
+        <v>0.004991689392707744</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -11907,7 +11907,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -11917,11 +11917,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Electricity by solar thermal</t>
+          <t>Electricity by solar photovoltaic</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>5.781892636926824e-06</v>
+        <v>0.0001412315744681418</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -11933,7 +11933,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -11943,11 +11943,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Electricity by solar thermal</t>
+          <t>Electricity by solar photovoltaic</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.0002023830590283706</v>
+        <v>0.0004632706091568247</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -11959,7 +11959,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -11973,7 +11973,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>1.57189172710456e-06</v>
+        <v>5.781892636926824e-06</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
@@ -11985,7 +11985,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -11999,7 +11999,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>2.265816426508705e-05</v>
+        <v>0.0002023830590283706</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -12011,7 +12011,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -12021,11 +12021,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Electricity by tide, wave, ocean</t>
+          <t>Electricity by solar thermal</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>7.4995863586978e-08</v>
+        <v>1.57189172710456e-06</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -12037,7 +12037,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -12047,11 +12047,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Electricity by tide, wave, ocean</t>
+          <t>Electricity by solar thermal</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>1.812705784425121e-05</v>
+        <v>2.265816426508705e-05</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -12063,7 +12063,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -12077,7 +12077,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>3.978838091980748e-07</v>
+        <v>7.4995863586978e-08</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
@@ -12089,7 +12089,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -12103,7 +12103,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1.812705784425121e-05</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -12115,7 +12115,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -12125,11 +12125,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Electricity by wind</t>
+          <t>Electricity by tide, wave, ocean</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.002574459447441928</v>
+        <v>3.978838091980748e-07</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -12141,7 +12141,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -12151,11 +12151,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Electricity by wind</t>
+          <t>Electricity by tide, wave, ocean</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.01526502959649972</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
@@ -12167,7 +12167,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -12181,7 +12181,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.0001751058206396409</v>
+        <v>0.002574459447441928</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -12193,7 +12193,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -12207,7 +12207,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.001577082488913786</v>
+        <v>0.01526502959649972</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -12219,7 +12219,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -12229,11 +12229,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Electricity nec</t>
+          <t>Electricity by wind</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>0.0001751058206396409</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
@@ -12245,7 +12245,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -12255,11 +12255,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Electricity nec</t>
+          <t>Electricity by wind</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.0002476113197245791</v>
+        <v>0.001577082488913786</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -12271,7 +12271,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -12285,7 +12285,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>2.789415361346499e-05</v>
+        <v>0</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -12297,7 +12297,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -12311,7 +12311,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>2.816362513459118e-05</v>
+        <v>0.0002476113197245791</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -12323,7 +12323,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -12333,23 +12333,23 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Fabricated metal products, except machinery and equipment (28)</t>
+          <t>Electricity nec</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>2.789415361346499e-05</v>
       </c>
       <c r="E68" t="n">
-        <v>0.3249344781605391</v>
+        <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>0.3154273852870779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -12359,11 +12359,11 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Glass and glass products</t>
+          <t>Electricity nec</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.08173033475287998</v>
+        <v>2.816362513459118e-05</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
@@ -12385,23 +12385,23 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Glass and glass products</t>
+          <t>Fabricated metal products, except machinery and equipment (28)</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.003063519910415851</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>0.1350980737190398</v>
+        <v>0.3249344781605391</v>
       </c>
       <c r="F70" t="n">
-        <v>0.08988970906257714</v>
+        <v>0.3097026100361647</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -12415,7 +12415,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.002625874208927872</v>
+        <v>0.08173033475287998</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
@@ -12427,7 +12427,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -12441,19 +12441,19 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.02199169649977092</v>
+        <v>0.003063519910415851</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>0.1350980737190398</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
+        <v>0.08988970906257714</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -12463,23 +12463,23 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Other business services (74)</t>
+          <t>Glass and glass products</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.02884338044418805</v>
+        <v>0.002625874208927872</v>
       </c>
       <c r="E73" t="n">
-        <v>0.1274059717763914</v>
+        <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -12489,17 +12489,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Other land transportation services</t>
+          <t>Glass and glass products</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.006057109893279482</v>
+        <v>0.02199169649977092</v>
       </c>
       <c r="E74" t="n">
-        <v>0.007016534431591046</v>
+        <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.035</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -12515,7 +12515,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Other non-ferrous metal products</t>
+          <t>Neodymium</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -12525,7 +12525,7 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>0.003714870872763483</v>
+        <v>0.002738804045443111</v>
       </c>
     </row>
     <row r="76">
@@ -12541,23 +12541,23 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Other non-metallic mineral products</t>
+          <t>Other business services (74)</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>0.02884338044418805</v>
       </c>
       <c r="E76" t="n">
-        <v>0.02123016211414608</v>
+        <v>0.1274059717763914</v>
       </c>
       <c r="F76" t="n">
-        <v>0.07426799999999999</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -12567,17 +12567,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Precious metals</t>
+          <t>Other land transportation services</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.0277214000916201</v>
+        <v>0.006057109893279482</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>0.007016534431591046</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="78">
@@ -12593,23 +12593,23 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Precious metals</t>
+          <t>Other non-metallic mineral products</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.001039088624585493</v>
+        <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>0.02123016211414608</v>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
+        <v>0.07426799999999999</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -12623,7 +12623,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.0008906473925018505</v>
+        <v>0.0277214000916201</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -12635,7 +12635,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -12649,7 +12649,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.007459171912202999</v>
+        <v>0.001039088624585493</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -12661,7 +12661,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -12671,11 +12671,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Raw silicon</t>
+          <t>Precious metals</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.03040485926127008</v>
+        <v>0.0008906473925018505</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
@@ -12687,7 +12687,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>EU27+UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -12697,11 +12697,11 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Raw silicon</t>
+          <t>Precious metals</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.003071197905178797</v>
+        <v>0.007459171912202999</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
@@ -12713,7 +12713,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -12727,7 +12727,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.002764078114660918</v>
+        <v>0.03040485926127008</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
@@ -12739,7 +12739,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>EU27+UK</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -12753,7 +12753,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.002149838533625158</v>
+        <v>0.003071197905178797</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
@@ -12765,7 +12765,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -12775,11 +12775,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Sea and coastal water transportation services</t>
+          <t>Raw silicon</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.05422555523507346</v>
+        <v>0.002764078114660918</v>
       </c>
       <c r="E85" t="n">
         <v>0</v>
@@ -12791,26 +12791,78 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Raw silicon</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.002149838533625158</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Sea and coastal water transportation services</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.05422555523507346</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
           <t>EU27+UK</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>Commodity</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>Sea and coastal water transportation services</t>
         </is>
       </c>
-      <c r="D86" t="n">
-        <v>0</v>
-      </c>
-      <c r="E86" t="n">
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" t="n">
         <v>0.007016534431591046</v>
       </c>
-      <c r="F86" t="n">
+      <c r="F88" t="n">
         <v>0.035</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Disaggregation of commodity Copper
</commit_message>
<xml_diff>
--- a/Add Sectors/new_activities.xlsx
+++ b/Add Sectors/new_activities.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="24468" yWindow="-108" windowWidth="24792" windowHeight="13320" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="indeces" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="units" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -452,7 +452,7 @@
   </sheetPr>
   <dimension ref="A1:I1105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -10230,6 +10230,17 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="D1:AH1" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:AH2" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$I$1:$I$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3:AH3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$F$1:$F$7</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10497,6 +10508,98 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="30">
+    <dataValidation sqref="A2" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A4" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A5" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A6" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A7" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A11" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A13" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A14" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A15" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A22" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A23" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A25" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A26" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A27" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A28" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A29" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A30" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+    <dataValidation sqref="A31" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$G$1:$G$12</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10572,6 +10675,98 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="30">
+    <dataValidation sqref="A2" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A4" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A5" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A6" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A7" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A11" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A13" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A14" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A15" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A22" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A23" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A25" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A26" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A27" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A28" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A29" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A30" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+    <dataValidation sqref="A31" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$H$1:$H$1105</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11007,7 +11202,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Copper ores and concentrates</t>
+          <t>Copper</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -11033,7 +11228,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Copper ores and concentrates</t>
+          <t>Copper</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -12867,6 +13062,278 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="90">
+    <dataValidation sqref="A2" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A4" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B4" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A5" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B5" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A6" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B6" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A7" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B7" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A11" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B11" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C11" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A13" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B13" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C13" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A14" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B14" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C14" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A15" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B15" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C15" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A22" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B22" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C22" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A23" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B23" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C23" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A25" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B25" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C25" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A26" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B26" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C26" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A27" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B27" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C27" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A28" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B28" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C28" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A29" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B29" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C29" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A30" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B30" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C30" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+    <dataValidation sqref="A31" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="B31" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="C31" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12958,6 +13425,17 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="D1:AH1" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:AH2" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$E$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3:AH3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+      <formula1>indeces!$B$1:$B$200</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12970,8 +13448,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -12986,36 +13464,21 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Production of offshore wind plants</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EUR</t>
+          <t>Production of onshore wind plants</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Production of photovoltaic plants</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>EUR</t>
+          <t>Production of offshore wind plants</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Production of onshore wind plants</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>EUR</t>
+          <t>Production of photovoltaic plants</t>
         </is>
       </c>
     </row>

</xml_diff>